<commit_message>
fix notification import user and add transactional insert database
</commit_message>
<xml_diff>
--- a/Implementation/public/file/excel/userImport.xlsx
+++ b/Implementation/public/file/excel/userImport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>username</t>
   </si>
@@ -75,6 +75,30 @@
   </si>
   <si>
     <t>lecturer</t>
+  </si>
+  <si>
+    <t>aldo</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>asdf@sad</t>
+  </si>
+  <si>
+    <t>andrianasd2</t>
+  </si>
+  <si>
+    <t>andriasdn2</t>
+  </si>
+  <si>
+    <t>adaff@ad</t>
   </si>
 </sst>
 </file>
@@ -389,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -422,22 +446,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>9870</v>
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -445,10 +469,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -460,9 +484,55 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>9870</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>9871</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>